<commit_message>
Search element in table by 'Артикул'. AddItem doesn't work yet...
</commit_message>
<xml_diff>
--- a/public/api/save/data.xlsx
+++ b/public/api/save/data.xlsx
@@ -401,19 +401,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
         <v>123</v>
       </c>
       <c r="B2" t="str">
         <v>aaa</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="str">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="str">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="str">
         <v>1</v>
       </c>
       <c r="F2" t="str">
@@ -421,83 +421,83 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>132123</v>
+      <c r="A3" t="str">
+        <v>1234</v>
       </c>
       <c r="B3" t="str">
-        <v>aaa</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>fff</v>
+      </c>
+      <c r="C3" t="str">
+        <v>45</v>
+      </c>
+      <c r="D3" t="str">
+        <v>32</v>
+      </c>
+      <c r="E3" t="str">
+        <v>42</v>
       </c>
       <c r="F3" t="str">
-        <v>aaa</v>
+        <v>aaaasd</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>777</v>
+      <c r="A4" t="str">
+        <v>231</v>
       </c>
       <c r="B4" t="str">
-        <v>aa</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
+        <v>asda</v>
+      </c>
+      <c r="C4" t="str">
+        <v>43</v>
+      </c>
+      <c r="D4" t="str">
+        <v>213</v>
       </c>
       <c r="E4" t="str">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F4" t="str">
-        <v>aa</v>
+        <v>aasda</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>7</v>
+        <v>3425</v>
       </c>
       <c r="B5" t="str">
-        <v>aaa</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
+        <v>aaaasd</v>
+      </c>
+      <c r="C5" t="str">
+        <v>123</v>
+      </c>
+      <c r="D5" t="str">
+        <v>23</v>
       </c>
       <c r="E5" t="str">
-        <v>3</v>
+        <v>3123</v>
       </c>
       <c r="F5" t="str">
-        <v>bb</v>
+        <v>asda</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v/>
+        <v>1231</v>
       </c>
       <c r="B6" t="str">
-        <v/>
+        <v>asdad</v>
       </c>
       <c r="C6" t="str">
-        <v/>
+        <v>42</v>
       </c>
       <c r="D6" t="str">
-        <v/>
+        <v>123</v>
       </c>
       <c r="E6" t="str">
-        <v/>
+        <v>24</v>
       </c>
       <c r="F6" t="str">
-        <v/>
+        <v>asdasdas</v>
       </c>
     </row>
   </sheetData>

</xml_diff>